<commit_message>
Instead of setting deadhead trips to Integer.MAX when not path is found, use the beeline distance and a factor to approximate those
</commit_message>
<xml_diff>
--- a/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config.xlsx
+++ b/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\integration-test\input\de\kelheim\kelheim-v3.0\25pct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E7F724-FD7D-45B4-A4FE-87F161F3F69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54284CDA-5AE6-483B-B493-8017841F15D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_info" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="maintenance_slots" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="98">
   <si>
     <t>location_id</t>
   </si>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t>short_6900</t>
+  </si>
+  <si>
+    <t>deadHeadTripBeelineDistanceFactor</t>
+  </si>
+  <si>
+    <t>The factor that is applied to travel the beeline distance at speed limit, if no path in the network is found for the dead head trip between two locations.</t>
   </si>
 </sst>
 </file>
@@ -730,11 +736,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -860,16 +866,13 @@
         <v>33</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>31</v>
+        <v>96</v>
+      </c>
+      <c r="C8" s="7">
+        <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -877,16 +880,16 @@
         <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="7">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -894,34 +897,34 @@
         <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C11" s="7">
         <f>15 * 60</f>
         <v>900</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="7">
-        <v>999</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -929,13 +932,16 @@
         <v>34</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="C12" s="7">
+        <v>999</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -943,33 +949,30 @@
         <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="7">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="C14" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -977,16 +980,16 @@
         <v>44</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="7">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -994,17 +997,16 @@
         <v>44</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7">
-        <f>2 * 60</f>
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1012,52 +1014,53 @@
         <v>44</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="7">
+        <f>2 * 60</f>
+        <v>120</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C18" s="7">
         <f>3 * 60</f>
         <v>180</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C19" s="7">
         <f>15000 * 1000</f>
         <v>15000000</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="7">
-        <v>100</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1065,16 +1068,16 @@
         <v>10</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="7">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1082,16 +1085,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1099,16 +1102,16 @@
         <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="7">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1116,20 +1119,37 @@
         <v>10</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="C23" s="7">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="7">
+        <v>200</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E23" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
+  <autoFilter ref="A1:E24" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Introduce solver instance id to specify output directory and file names
</commit_message>
<xml_diff>
--- a/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config.xlsx
+++ b/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\integration-test\input\de\kelheim\kelheim-v3.0\25pct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54284CDA-5AE6-483B-B493-8017841F15D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F44389F-72FE-4A36-9E8C-42B36C0083D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
@@ -264,9 +264,6 @@
     <t>instanceId</t>
   </si>
   <si>
-    <t>rss001</t>
-  </si>
-  <si>
     <t>Id of the rssched instance to solve, which is configured in this config file.</t>
   </si>
   <si>
@@ -337,6 +334,9 @@
   </si>
   <si>
     <t>The factor that is applied to travel the beeline distance at speed limit, if no path in the network is found for the dead head trip between two locations.</t>
+  </si>
+  <si>
+    <t>it_config</t>
   </si>
 </sst>
 </file>
@@ -740,7 +740,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -777,11 +777,11 @@
         <v>72</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -792,7 +792,7 @@
         <v>71</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>23</v>
@@ -803,10 +803,10 @@
         <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>24</v>
@@ -820,7 +820,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>25</v>
@@ -866,13 +866,13 @@
         <v>33</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="7">
         <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1200,7 +1200,7 @@
         <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -1217,7 +1217,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>600</v>
@@ -1255,42 +1255,42 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1330,10 +1330,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1341,10 +1341,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -1352,10 +1352,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -1374,10 +1374,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1407,10 +1407,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -1418,10 +1418,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -1429,10 +1429,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -1451,10 +1451,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17">
         <v>2</v>

</xml_diff>

<commit_message>
Remove dependency on matsim run output config file
The keys in the matsim config file change over the time and become deprecated or defunct. Since this requires to have a reader from the specific matsim version, incompatibilities arise. To avoid this the dependency is removed, the only downside is that now the network CRS has to be provided as further input.
</commit_message>
<xml_diff>
--- a/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config.xlsx
+++ b/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\integration-test\input\de\kelheim\kelheim-v3.0\25pct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F44389F-72FE-4A36-9E8C-42B36C0083D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86D825F-BC53-488E-A44C-C1A150108DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_info" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="maintenance_slots" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="101">
   <si>
     <t>location_id</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t>it_config</t>
+  </si>
+  <si>
+    <t>EPSG:25832</t>
+  </si>
+  <si>
+    <t>networkCrs</t>
+  </si>
+  <si>
+    <t>The coordinate reference system of the network</t>
   </si>
 </sst>
 </file>
@@ -736,11 +745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -831,16 +840,13 @@
         <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>29</v>
+        <v>99</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -848,17 +854,16 @@
         <v>33</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C7" s="7">
-        <f>90 / 3.6</f>
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -866,13 +871,17 @@
         <v>33</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="C8" s="7">
-        <v>5</v>
+        <f>90 / 3.6</f>
+        <v>25</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -880,16 +889,13 @@
         <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>31</v>
+        <v>95</v>
+      </c>
+      <c r="C9" s="7">
+        <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -897,16 +903,16 @@
         <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7">
+        <v>17</v>
+      </c>
+      <c r="C10" s="7" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -914,34 +920,34 @@
         <v>33</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C12" s="7">
         <f>15 * 60</f>
         <v>900</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="7">
-        <v>999</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -949,13 +955,16 @@
         <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="C13" s="7">
+        <v>999</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -963,33 +972,30 @@
         <v>34</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="7">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="C15" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -997,16 +1003,16 @@
         <v>44</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="7">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1014,17 +1020,16 @@
         <v>44</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="7">
-        <f>2 * 60</f>
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,52 +1037,53 @@
         <v>44</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="7">
+        <f>2 * 60</f>
+        <v>120</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C19" s="7">
         <f>3 * 60</f>
         <v>180</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C20" s="7">
         <f>15000 * 1000</f>
         <v>15000000</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="7">
-        <v>100</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1085,16 +1091,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="7">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1102,16 +1108,16 @@
         <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="7">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1119,16 +1125,16 @@
         <v>10</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="7">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1136,20 +1142,37 @@
         <v>10</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="C24" s="7">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="7">
+        <v>200</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E24" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
+  <autoFilter ref="A1:E25" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>